<commit_message>
added important files folder
</commit_message>
<xml_diff>
--- a/02_output/12_statistical_tests/phi_mixed_model_tests.xlsx
+++ b/02_output/12_statistical_tests/phi_mixed_model_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f304f79f068e311c/Universitaet/MASTER/MasterThesis/11_Data_Analysis_MA/02_output/12_statistical_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_8B72B13000D96F86106438FA5F3D0122F21D9C32" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBA39FCC-5D1E-4C9F-B3B2-271530569B2B}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_8B72B13000D96F86106438FA5F3D0122F21D9C32" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15919DB2-5047-497E-9988-D44B77CB6342}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="71895" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -458,8 +458,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1704,7 +1704,7 @@
         <v>0.683075092457471</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0.73716282430202595</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1832,7 +1832,7 @@
   <autoFilter ref="A1:T22" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="phi_total_no_yield"/>
+        <filter val="phi_total"/>
       </filters>
     </filterColumn>
     <filterColumn colId="2">

</xml_diff>